<commit_message>
Agregado de mas modulos
Agregado Leds, Switchs y Alimentación
</commit_message>
<xml_diff>
--- a/BOM_nRF51822.xlsx
+++ b/BOM_nRF51822.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
   <si>
     <t>Qty</t>
   </si>
@@ -130,6 +130,75 @@
   </si>
   <si>
     <t>http://www.digikey.com/scripts/DkSearch/dksus.dll?lang=en&amp;vendor=0&amp;WT.z_cid=ref_findchips0311_dkc_buynow&amp;mpart=BAT-HLD-001&amp;cur=USD</t>
+  </si>
+  <si>
+    <t>2450AT18B100E</t>
+  </si>
+  <si>
+    <t>ANT</t>
+  </si>
+  <si>
+    <t>609-2450AT18B100E</t>
+  </si>
+  <si>
+    <t>http://mx.mouser.com/search/ProductDetail.aspx?qs=yCnrNFeXz%252bh5MFsFIXGZGA==&amp;utm_source=findchips&amp;utm_medium=aggregator&amp;utm_campaign=609-2450AT18B100E&amp;utm_term=2450AT18B100</t>
+  </si>
+  <si>
+    <t>712-1006-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/2450AT18B100E/712-1006-1-ND/1560835</t>
+  </si>
+  <si>
+    <t>CHIP_ANTENNA</t>
+  </si>
+  <si>
+    <t>BAT165</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>BAT 165 E6327</t>
+  </si>
+  <si>
+    <t>726-BAT165E6327</t>
+  </si>
+  <si>
+    <t>http://mx.mouser.com/search/ProductDetail.aspx?qs=mzcOS1kGbgcQqWsJMFtrug==&amp;utm_source=findchips&amp;utm_medium=aggregator&amp;utm_campaign=726-BAT165E6327&amp;utm_term=BAT165</t>
+  </si>
+  <si>
+    <t>BAT 165 E6327CT-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/BAT%20165%20E6327/BAT%20165%20E6327CT-ND/3819504</t>
+  </si>
+  <si>
+    <t>BALUM</t>
+  </si>
+  <si>
+    <t>2450BM14A0002T</t>
+  </si>
+  <si>
+    <t>609-2450BM14A0002T</t>
+  </si>
+  <si>
+    <t>http://mx.mouser.com/search/ProductDetail.aspx?qs=yCnrNFeXz%252bjc2NrpGmrycg==&amp;utm_source=findchips&amp;utm_medium=aggregator&amp;utm_campaign=609-2450BM14A0002T&amp;utm_term=2450BM14A0002</t>
+  </si>
+  <si>
+    <t>SWITCH</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>SKQGADE010</t>
+  </si>
+  <si>
+    <t>688-SKQGAD</t>
+  </si>
+  <si>
+    <t>http://mx.mouser.com/search/ProductDetail.aspx?qs=N5Jky1br14PCAY42dbciFw==&amp;utm_source=findchips&amp;utm_medium=aggregator&amp;utm_campaign=688-SKQGAD&amp;utm_term=SKQGADE010</t>
   </si>
 </sst>
 </file>
@@ -190,14 +259,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -500,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:M10"/>
+  <dimension ref="B3:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,56 +589,56 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -595,13 +664,13 @@
       <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>1674</v>
       </c>
       <c r="J5">
         <v>1.62</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="M5" t="s">
@@ -618,13 +687,13 @@
       <c r="H6" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>1759</v>
       </c>
       <c r="J6">
         <v>2.54</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="M6" t="s">
@@ -641,13 +710,13 @@
       <c r="H7" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>3766</v>
       </c>
       <c r="J7">
         <v>3.65</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="M7" t="s">
@@ -676,13 +745,13 @@
       <c r="H8" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <v>19369</v>
       </c>
       <c r="J8">
         <v>0.32</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="3" t="s">
         <v>32</v>
       </c>
       <c r="M8" t="s">
@@ -699,13 +768,13 @@
       <c r="H9" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>26890</v>
       </c>
       <c r="J9">
         <v>0.35099999999999998</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="3" t="s">
         <v>35</v>
       </c>
       <c r="M9" t="s">
@@ -722,16 +791,202 @@
       <c r="H10" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>37903</v>
       </c>
       <c r="J10">
         <v>0.27</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="3" t="s">
         <v>37</v>
       </c>
       <c r="M10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="4">
+        <v>5517</v>
+      </c>
+      <c r="J11">
+        <v>1.21</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="4">
+        <v>10828</v>
+      </c>
+      <c r="J12">
+        <v>0.94</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="4">
+        <v>9000</v>
+      </c>
+      <c r="J13">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" t="s">
+        <v>50</v>
+      </c>
+      <c r="I14" s="4">
+        <v>1619</v>
+      </c>
+      <c r="J14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="4">
+        <v>3773</v>
+      </c>
+      <c r="J15">
+        <v>1.91</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="4">
+        <v>642</v>
+      </c>
+      <c r="J16">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M16" t="s">
         <v>27</v>
       </c>
     </row>
@@ -746,6 +1001,12 @@
     <hyperlink ref="L8" r:id="rId4"/>
     <hyperlink ref="L9" r:id="rId5"/>
     <hyperlink ref="L10" r:id="rId6"/>
+    <hyperlink ref="L11" r:id="rId7"/>
+    <hyperlink ref="L12" r:id="rId8"/>
+    <hyperlink ref="L13" r:id="rId9"/>
+    <hyperlink ref="L14" r:id="rId10"/>
+    <hyperlink ref="L15" r:id="rId11"/>
+    <hyperlink ref="L16" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>